<commit_message>
Expand instr to miniRV: create module NPC
</commit_message>
<xml_diff>
--- a/数据通路_控制信号表.xlsx
+++ b/数据通路_控制信号表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\CPU_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAA16BB-BEB7-4369-8DD5-928588CE5064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B12B6E-B63B-49EF-9F02-A94CD08C6564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据通路表" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="142">
   <si>
     <t>所属单元</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>npc_op</t>
-  </si>
-  <si>
-    <t>isTrue</t>
   </si>
   <si>
     <t>daddr</t>
@@ -237,16 +234,10 @@
   </si>
   <si>
     <t>0110011</t>
-  </si>
-  <si>
-    <t>0110011</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>0010011</t>
-  </si>
-  <si>
-    <t>0010011</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -279,6 +270,268 @@
   </si>
   <si>
     <t>1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC.npc</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC.pc</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>执行操作</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>加法</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>减法</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>位与</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>位或</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>位异或</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>左移</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>左移不分逻辑/算术</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>逻辑右移</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>高位永远补0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>高位按照原符号位补</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>算数右移</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>相等</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>不相等</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>小于</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>大于等于</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0010</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0011</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0100</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0101</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0110</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0111</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1010</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1101</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>X000</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>X111</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>X110</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>X100</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>X001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>X101</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>X010</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXXX</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>将 20 位立即数加载到寄存器的高位​​，低位补零</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接跳转，跳转范围pc+-1MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>pc+4</t>
+  </si>
+  <si>
+    <t>pc+4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctrl_ALU[3:0]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctrl_NPC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctrl_WriteReg</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>可能pc+offset</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctrl_WriteDRAM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制某一个器件的输入选择
+（给到前置MUX）</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要的控制信号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>器件</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DRAM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>IROM</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制某一个器件的输出选择
+（给到器件本身，作为输入）
+简称：控后信号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制某一个器件的输入选择
+（给到前置MUX）
+简称：控前信号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>控中信号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>控后信号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctrl_ALU</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制某一个器件本身的内容是否更改
+（给到器件本身，作为输入，1位）
+简称：控中信号</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -331,7 +584,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -476,11 +729,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF1F2329"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF1F2329"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF1F2329"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF1F2329"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF1F2329"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF1F2329"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF1F2329"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF1F2329"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF1F2329"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF1F2329"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF1F2329"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF1F2329"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF1F2329"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -527,6 +861,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -846,13 +1228,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:T29"/>
+  <dimension ref="B2:U29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,28 +1246,29 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
-      <c r="P2" s="11" t="s">
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="11"/>
+      <c r="T2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U2" s="11"/>
+    </row>
+    <row r="3" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -895,34 +1280,35 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="17"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="11"/>
+      <c r="N3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="O3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="13"/>
+      <c r="Q3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="11"/>
+      <c r="T3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="11"/>
-    </row>
-    <row r="4" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -938,60 +1324,67 @@
       <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="T4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="T4" s="3" t="s">
+    </row>
+    <row r="5" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -1003,18 +1396,23 @@
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -1026,18 +1424,23 @@
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-    </row>
-    <row r="7" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -1049,18 +1452,23 @@
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-    </row>
-    <row r="8" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U7" s="3"/>
+    </row>
+    <row r="8" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="18"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1072,18 +1480,23 @@
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
-    </row>
-    <row r="9" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1095,18 +1508,19 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1118,18 +1532,19 @@
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U10" s="3"/>
+    </row>
+    <row r="11" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="3"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1141,18 +1556,19 @@
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1164,18 +1580,19 @@
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1187,18 +1604,19 @@
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-    </row>
-    <row r="14" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1210,18 +1628,19 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-    </row>
-    <row r="15" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
       <c r="E15" s="3"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1233,18 +1652,19 @@
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-    </row>
-    <row r="16" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="1"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1256,18 +1676,19 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U16" s="3"/>
+    </row>
+    <row r="17" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="1"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1279,18 +1700,19 @@
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U17" s="3"/>
+    </row>
+    <row r="18" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="1"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1302,18 +1724,19 @@
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U18" s="3"/>
+    </row>
+    <row r="19" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="1"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1325,18 +1748,19 @@
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
-    </row>
-    <row r="20" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U19" s="3"/>
+    </row>
+    <row r="20" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="1"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1348,18 +1772,19 @@
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="1"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1367,114 +1792,119 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="4"/>
+      <c r="Q21" s="3"/>
       <c r="R21" s="4"/>
-      <c r="S21" s="3"/>
+      <c r="S21" s="4"/>
       <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="1"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="1"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="5"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="3"/>
+      <c r="S22" s="1"/>
       <c r="T22" s="3"/>
-    </row>
-    <row r="23" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="1"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="1"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="5"/>
       <c r="R23" s="1"/>
-      <c r="S23" s="3"/>
+      <c r="S23" s="1"/>
       <c r="T23" s="3"/>
-    </row>
-    <row r="24" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="1"/>
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="1"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="1"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="5"/>
       <c r="R24" s="1"/>
-      <c r="S24" s="3"/>
+      <c r="S24" s="1"/>
       <c r="T24" s="3"/>
-    </row>
-    <row r="25" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U24" s="3"/>
+    </row>
+    <row r="25" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="1"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="1"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="5"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="3"/>
+      <c r="S25" s="1"/>
       <c r="T25" s="3"/>
-    </row>
-    <row r="26" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U25" s="3"/>
+    </row>
+    <row r="26" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="1"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1482,22 +1912,23 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="1"/>
+      <c r="Q26" s="3"/>
       <c r="R26" s="1"/>
-      <c r="S26" s="3"/>
+      <c r="S26" s="1"/>
       <c r="T26" s="3"/>
-    </row>
-    <row r="27" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U26" s="3"/>
+    </row>
+    <row r="27" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="1"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -1509,18 +1940,19 @@
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
-    </row>
-    <row r="28" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U27" s="3"/>
+    </row>
+    <row r="28" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="1"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="1"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -1532,18 +1964,19 @@
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
-    </row>
-    <row r="29" spans="2:20" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="U28" s="3"/>
+    </row>
+    <row r="29" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="1"/>
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="1"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="1"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -1551,22 +1984,23 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="1"/>
       <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1578,483 +2012,887 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:K27"/>
+  <dimension ref="A2:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="38.7265625" customWidth="1"/>
     <col min="5" max="5" width="38.1796875" customWidth="1"/>
+    <col min="13" max="13" width="14.6328125" customWidth="1"/>
+    <col min="14" max="14" width="16.1796875" customWidth="1"/>
+    <col min="15" max="15" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+    </row>
+    <row r="3" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="16"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="O3" s="20"/>
+      <c r="P3" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="20"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="J4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
       <c r="C5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>70</v>
+        <v>31</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>68</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B6" s="14"/>
       <c r="C6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>70</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D6" s="29"/>
       <c r="E6" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>69</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D7" s="29"/>
       <c r="E7" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>69</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D8" s="29"/>
       <c r="E8" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>69</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D9" s="29"/>
       <c r="E9" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
       <c r="B10" s="14"/>
       <c r="C10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>69</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D10" s="29"/>
       <c r="E10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
       <c r="B11" s="14"/>
       <c r="C11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D13" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="E13" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B16" s="14"/>
       <c r="C16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D16" s="29"/>
       <c r="E16" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B17" s="14"/>
       <c r="C17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D17" s="29"/>
       <c r="E17" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B18" s="14"/>
       <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E21" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B23" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B23" s="14"/>
-      <c r="C23" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="E23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B24" s="14"/>
       <c r="C24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B25" s="14"/>
       <c r="C25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B26" s="14"/>
+      <c r="C26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
+      <c r="D27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="2:11" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="M28" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" t="s">
+        <v>128</v>
+      </c>
+      <c r="I34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" t="s">
+        <v>126</v>
+      </c>
+      <c r="H35" t="s">
+        <v>138</v>
+      </c>
+      <c r="I35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>136</v>
+      </c>
+      <c r="G36" t="s">
+        <v>136</v>
+      </c>
+      <c r="H36" t="s">
+        <v>137</v>
+      </c>
+      <c r="I36" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:K2"/>
+  <mergeCells count="15">
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="D13:D19"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="J2:S2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="B13:B19"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Expand instr to miniRV-2
Upgrade module control and npc, create module alu_simple for cauculation in npc module.
</commit_message>
<xml_diff>
--- a/数据通路_控制信号表.xlsx
+++ b/数据通路_控制信号表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\CPU_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B12B6E-B63B-49EF-9F02-A94CD08C6564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4144026D-AF1E-4285-8CA7-D06590FF5AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="数据通路表" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="143">
   <si>
     <t>所属单元</t>
   </si>
@@ -200,10 +200,6 @@
   </si>
   <si>
     <t>指令</t>
-  </si>
-  <si>
-    <t>funct
-{funct7[6], funct3}</t>
   </si>
   <si>
     <t>控制信号</t>
@@ -532,6 +528,15 @@
     <t>控制某一个器件本身的内容是否更改
 （给到器件本身，作为输入，1位）
 简称：控中信号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>funct
+{funct7[6], funct3}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>beq</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -576,12 +581,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="19">
@@ -814,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -845,32 +856,53 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -878,9 +910,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,26 +919,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,7 +1247,7 @@
   </sheetPr>
   <dimension ref="B2:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1240,33 +1257,33 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11" t="s">
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="11"/>
+      <c r="U2" s="15"/>
     </row>
     <row r="3" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1275,38 +1292,38 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="12"/>
+      <c r="H3" s="16"/>
       <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
       <c r="N3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="11" t="s">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11" t="s">
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="11"/>
+      <c r="U3" s="15"/>
     </row>
     <row r="4" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1324,11 +1341,11 @@
       <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>19</v>
@@ -1375,14 +1392,14 @@
         <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="3"/>
@@ -1403,14 +1420,14 @@
         <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="3"/>
@@ -1431,14 +1448,14 @@
         <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="18"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="3"/>
@@ -1459,14 +1476,14 @@
         <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="3"/>
@@ -1487,14 +1504,14 @@
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="3"/>
@@ -1518,7 +1535,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="3"/>
@@ -1542,7 +1559,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="3"/>
@@ -1566,7 +1583,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="18"/>
+      <c r="G12" s="10"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="3"/>
@@ -1590,7 +1607,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="3"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="18"/>
+      <c r="G13" s="10"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="3"/>
@@ -1614,7 +1631,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="3"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="10"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="3"/>
@@ -1638,7 +1655,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="3"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="18"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="3"/>
@@ -1662,7 +1679,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="18"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="3"/>
@@ -1686,7 +1703,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="18"/>
+      <c r="G17" s="10"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="3"/>
@@ -1710,7 +1727,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="18"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="3"/>
@@ -1734,7 +1751,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="10"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="3"/>
@@ -1758,7 +1775,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="18"/>
+      <c r="G20" s="10"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="3"/>
@@ -1782,7 +1799,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="3"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="18"/>
+      <c r="G21" s="10"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="3"/>
@@ -1806,7 +1823,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="18"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="3"/>
@@ -1830,7 +1847,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="18"/>
+      <c r="G23" s="10"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="3"/>
@@ -1854,7 +1871,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="18"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="3"/>
@@ -1878,7 +1895,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="18"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="3"/>
@@ -1902,7 +1919,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="18"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="3"/>
@@ -1926,7 +1943,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="18"/>
+      <c r="G27" s="10"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="3"/>
@@ -1950,7 +1967,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="3"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="10"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="3"/>
@@ -1974,7 +1991,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="18"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="3"/>
@@ -2014,866 +2031,867 @@
   </sheetPr>
   <dimension ref="A2:S36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.7265625" customWidth="1"/>
     <col min="5" max="5" width="38.1796875" customWidth="1"/>
+    <col min="6" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.6328125" customWidth="1"/>
     <col min="14" max="14" width="16.1796875" customWidth="1"/>
     <col min="15" max="15" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
     </row>
     <row r="3" spans="1:19" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-      <c r="F3" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21" t="s">
+      <c r="F3" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="20"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="27"/>
+      <c r="P3" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="27"/>
     </row>
     <row r="4" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
       <c r="J4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="L5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="19"/>
+      <c r="C6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="K5" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O5" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="19"/>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N7" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="O7" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="19"/>
+      <c r="C8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" s="3" t="s">
+      <c r="O8" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="19"/>
+      <c r="C9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="14"/>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
-      <c r="C9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="O9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="29"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="O10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="K11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="O11" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="8" t="s">
+      <c r="L12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="J13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="O13" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="19"/>
+      <c r="C14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="O14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="19"/>
+      <c r="C15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="19"/>
+      <c r="C16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="19"/>
+      <c r="C17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L13" s="3" t="s">
+      <c r="J17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O13" s="3" t="s">
+      <c r="O17" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="19"/>
+      <c r="C18" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="O18" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="19"/>
+      <c r="C19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
-      <c r="C15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="14"/>
-      <c r="C17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
-      <c r="C18" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="14"/>
-      <c r="C19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="O19" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="K20" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N20" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="O20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C23" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L22" s="3" t="s">
+      <c r="E23" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M22" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N22" s="3" t="s">
+      <c r="M23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B24" s="19"/>
+      <c r="C24" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N23" s="3" t="s">
+      <c r="M24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B25" s="19"/>
+      <c r="C25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="23"/>
+      <c r="E25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="M25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B26" s="19"/>
+      <c r="C26" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L26" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B24" s="14"/>
-      <c r="C24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B25" s="14"/>
-      <c r="C25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B26" s="14"/>
-      <c r="C26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="M26" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M27" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="O27" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" t="s">
         <v>131</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>132</v>
       </c>
-      <c r="G34" t="s">
-        <v>133</v>
-      </c>
       <c r="H34" t="s">
+        <v>127</v>
+      </c>
+      <c r="I34" t="s">
         <v>128</v>
-      </c>
-      <c r="I34" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="35" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="5:9" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
+        <v>135</v>
+      </c>
+      <c r="G36" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" t="s">
         <v>136</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>136</v>
-      </c>
-      <c r="H36" t="s">
-        <v>137</v>
-      </c>
-      <c r="I36" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expand instr to miniRV-4
(1) Finish the top file "single_CPU", edit a lot of name of variables.
(2) Use IP core templates in "single_CPU".
</commit_message>
<xml_diff>
--- a/数据通路_控制信号表.xlsx
+++ b/数据通路_控制信号表.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawei\Documents\GitHub\CPU_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5426CE7-6E60-4309-801E-C3A06903C854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D0083A-D7B0-45A3-A1F8-E6BAD4D7A761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12780" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="数据通路表" sheetId="2" r:id="rId1"/>
-    <sheet name="控制信号表" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="模块信号表" sheetId="4" r:id="rId1"/>
+    <sheet name="数据通路表" sheetId="2" r:id="rId2"/>
+    <sheet name="控制信号表" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="186">
   <si>
     <t>所属单元</t>
   </si>
@@ -627,15 +627,146 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>输入输出线</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>规范</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1、模块起名字使用【全大写】或【大驼峰】规范，比如ALU，RegFile</t>
+    <t>A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctrl_ALU_output</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>输入（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>控制</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）/输出</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[31:0]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>位宽范围</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>input</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>output</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[3:0]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>信号名称</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入输出信号</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegFile</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>clk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>rst</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>作用及功能描述</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>wr_reg_en</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>wr_reg_addr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>wr_wdata</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>规范说明
+1、模块起名字使用【全大写】或【大驼峰】规范，比如ALU，RegFile；
+2、信号起名字使用【全小写】或【蛇形命名法】规范，比如result，pc_add4，ALU中的标志位除外；
+3、特别地，控制信号名字</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>在控制模块中</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>遵循“ctrl_模块名_控制信号类型”的样式，其中模块名规范参照第1条，控制信号类型分为：控前信号（标识input）、控中信号（比如标识write）、控后信号（标识output）；
+4、rst信号为高有效。</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -643,7 +774,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -684,6 +815,30 @@
       <color rgb="FF7CA668"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -867,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -892,6 +1047,36 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -913,6 +1098,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -925,47 +1122,20 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1280,6 +1450,186 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDFC25C-9253-4547-9B42-25F2705FC719}">
+  <dimension ref="A4:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:7" ht="124" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+    </row>
+    <row r="5" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A4:G4"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3ACD1D0-60FC-4217-9D30-DACABEF04162}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1296,33 +1646,33 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="10" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10" t="s">
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10" t="s">
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="10"/>
+      <c r="U2" s="20"/>
     </row>
     <row r="3" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -1331,38 +1681,38 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="11"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
       <c r="N3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="10" t="s">
+      <c r="P3" s="23"/>
+      <c r="Q3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10" t="s">
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="10"/>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -2063,7 +2413,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96948F25-66D6-464E-B3EA-4F0CC018BDAF}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2090,1319 +2440,1314 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="28"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="18" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="18" t="s">
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
     </row>
     <row r="4" spans="1:17" ht="31" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="20" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="32" t="s">
+      <c r="G5" s="27"/>
+      <c r="H5" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="19"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="8">
         <v>1</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="P6" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="8">
         <v>1</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="M7" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="P7" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="25" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="19" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="8">
         <v>1</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L8" s="19" t="s">
+      <c r="L8" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="19" t="s">
+      <c r="M8" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N8" s="19" t="s">
+      <c r="N8" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="O8" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="P8" s="19" t="s">
+      <c r="P8" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="Q8" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="25" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="19" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="19" t="s">
+      <c r="M9" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N9" s="19" t="s">
+      <c r="N9" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O9" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="P9" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="Q9" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="25" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="24"/>
+      <c r="E10" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="8">
         <v>1</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="N10" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="O10" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="P10" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="Q10" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="8">
         <v>1</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="O11" s="19" t="s">
+      <c r="O11" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="P11" s="19" t="s">
+      <c r="P11" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q11" s="19" t="s">
+      <c r="Q11" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="29"/>
+      <c r="C12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="24"/>
+      <c r="E12" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="8">
         <v>1</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N12" s="19" t="s">
+      <c r="N12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="19" t="s">
+      <c r="O12" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="P12" s="19" t="s">
+      <c r="P12" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q12" s="19" t="s">
+      <c r="Q12" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="19" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="8">
         <v>1</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L13" s="19" t="s">
+      <c r="L13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M13" s="19" t="s">
+      <c r="M13" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N13" s="19" t="s">
+      <c r="N13" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="O13" s="19" t="s">
+      <c r="O13" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="P13" s="19" t="s">
+      <c r="P13" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q13" s="19" t="s">
+      <c r="Q13" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="8">
         <v>0</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M14" s="19" t="s">
+      <c r="M14" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N14" s="19" t="s">
+      <c r="N14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O14" s="19" t="s">
+      <c r="O14" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q14" s="19" t="s">
+      <c r="Q14" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="25" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="19" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="8">
         <v>0</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K15" s="19" t="s">
+      <c r="K15" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N15" s="19" t="s">
+      <c r="N15" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="O15" s="19" t="s">
+      <c r="O15" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="P15" s="19" t="s">
+      <c r="P15" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q15" s="19" t="s">
+      <c r="Q15" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="25" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="19" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="8">
         <v>0</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I16" s="20" t="s">
+      <c r="I16" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M16" s="19" t="s">
+      <c r="M16" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N16" s="19" t="s">
+      <c r="N16" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="O16" s="19" t="s">
+      <c r="O16" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="P16" s="19" t="s">
+      <c r="P16" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q16" s="19" t="s">
+      <c r="Q16" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="25" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="19" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="8">
         <v>0</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H17" s="30" t="s">
+      <c r="H17" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M17" s="19" t="s">
+      <c r="M17" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="N17" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="O17" s="19" t="s">
+      <c r="O17" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="P17" s="19" t="s">
+      <c r="P17" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q17" s="19" t="s">
+      <c r="Q17" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="25" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="19" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="8">
         <v>0</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="H18" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L18" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M18" s="19" t="s">
+      <c r="M18" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N18" s="19" t="s">
+      <c r="N18" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="O18" s="19" t="s">
+      <c r="O18" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="P18" s="19" t="s">
+      <c r="P18" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q18" s="19" t="s">
+      <c r="Q18" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="25" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="19" t="s">
+      <c r="D19" s="24"/>
+      <c r="E19" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L19" s="19" t="s">
+      <c r="L19" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="19" t="s">
+      <c r="M19" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N19" s="19" t="s">
+      <c r="N19" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="O19" s="19" t="s">
+      <c r="O19" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q19" s="19" t="s">
+      <c r="Q19" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="25" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="19" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="8">
         <v>0</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="19" t="s">
+      <c r="L20" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N20" s="19" t="s">
+      <c r="N20" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="O20" s="19" t="s">
+      <c r="O20" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="P20" s="19" t="s">
+      <c r="P20" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q20" s="19" t="s">
+      <c r="Q20" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L21" s="19" t="s">
+      <c r="L21" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M21" s="19" t="s">
+      <c r="M21" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N21" s="19" t="s">
+      <c r="N21" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="O21" s="19" t="s">
+      <c r="O21" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="P21" s="19" t="s">
+      <c r="P21" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q21" s="19" t="s">
+      <c r="Q21" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="8">
         <v>0</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L22" s="19" t="s">
+      <c r="L22" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M22" s="19" t="s">
+      <c r="M22" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N22" s="19" t="s">
+      <c r="N22" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O22" s="19" t="s">
+      <c r="O22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P22" s="19" t="s">
+      <c r="P22" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="Q22" s="19" t="s">
+      <c r="Q22" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="24" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="8">
         <v>0</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="H23" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L23" s="19" t="s">
+      <c r="L23" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="M23" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="N23" s="19" t="s">
+      <c r="N23" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="O23" s="19" t="s">
+      <c r="O23" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="P23" s="19" t="s">
+      <c r="P23" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q23" s="19" t="s">
+      <c r="Q23" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="8">
         <v>1</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H24" s="30" t="s">
+      <c r="H24" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I24" s="30" t="s">
+      <c r="I24" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N24" s="19" t="s">
+      <c r="N24" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O24" s="19" t="s">
+      <c r="O24" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P24" s="19" t="s">
+      <c r="P24" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="Q24" s="19" t="s">
+      <c r="Q24" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="25" t="s">
+      <c r="B25" s="29"/>
+      <c r="C25" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="19" t="s">
+      <c r="D25" s="24"/>
+      <c r="E25" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="8">
         <v>1</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="H25" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I25" s="30" t="s">
+      <c r="I25" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L25" s="19" t="s">
+      <c r="L25" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M25" s="19" t="s">
+      <c r="M25" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N25" s="19" t="s">
+      <c r="N25" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O25" s="19" t="s">
+      <c r="O25" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P25" s="19" t="s">
+      <c r="P25" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="Q25" s="19" t="s">
+      <c r="Q25" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="25" t="s">
+      <c r="B26" s="29"/>
+      <c r="C26" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="19" t="s">
+      <c r="D26" s="24"/>
+      <c r="E26" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="8">
         <v>1</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H26" s="30" t="s">
+      <c r="H26" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I26" s="30" t="s">
+      <c r="I26" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K26" s="19" t="s">
+      <c r="K26" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L26" s="19" t="s">
+      <c r="L26" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M26" s="19" t="s">
+      <c r="M26" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N26" s="19" t="s">
+      <c r="N26" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O26" s="19" t="s">
+      <c r="O26" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P26" s="19" t="s">
+      <c r="P26" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="Q26" s="19" t="s">
+      <c r="Q26" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="25" t="s">
+      <c r="B27" s="29"/>
+      <c r="C27" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="19" t="s">
+      <c r="D27" s="24"/>
+      <c r="E27" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="8">
         <v>1</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="H27" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I27" s="30" t="s">
+      <c r="I27" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="J27" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K27" s="19" t="s">
+      <c r="K27" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L27" s="19" t="s">
+      <c r="L27" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M27" s="19" t="s">
+      <c r="M27" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N27" s="19" t="s">
+      <c r="N27" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O27" s="19" t="s">
+      <c r="O27" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="P27" s="19" t="s">
+      <c r="P27" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q27" s="19" t="s">
+      <c r="Q27" s="11" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="H28" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="I28" s="20" t="s">
+      <c r="I28" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L28" s="19" t="s">
+      <c r="L28" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M28" s="19" t="s">
+      <c r="M28" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N28" s="19" t="s">
+      <c r="N28" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="O28" s="19" t="s">
+      <c r="O28" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="P28" s="19" t="s">
+      <c r="P28" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q28" s="19" t="s">
+      <c r="Q28" s="11" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H29" s="30" t="s">
+      <c r="H29" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="I29" s="20" t="s">
+      <c r="I29" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="L29" s="19" t="s">
+      <c r="L29" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="M29" s="19" t="s">
+      <c r="M29" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N29" s="19" t="s">
+      <c r="N29" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="O29" s="19" t="s">
+      <c r="O29" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="P29" s="19" t="s">
+      <c r="P29" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="Q29" s="19" t="s">
+      <c r="Q29" s="11" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="E30" s="29"/>
+      <c r="E30" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="F2:Q2"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:B13"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B2:B4"/>
@@ -3410,55 +3755,18 @@
     <mergeCell ref="D6:D13"/>
     <mergeCell ref="D14:D20"/>
     <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="F2:Q2"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:B13"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="F3:I3"/>
-    <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="J3:M3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDFC25C-9253-4547-9B42-25F2705FC719}">
-  <dimension ref="A3:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>